<commit_message>
added priorities, estimates, and assignments for sprint 1
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\norton402\Documents\Cita 450\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E633DA07-1CD5-4712-BC00-DFEA48A333AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94F30DD-8E44-4146-BAC0-798B1BE62C5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2160" windowWidth="14400" windowHeight="7360" xr2:uid="{4E35D11C-B807-4C4A-A7E5-3891EF9C7B2D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4E35D11C-B807-4C4A-A7E5-3891EF9C7B2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t xml:space="preserve">User Story </t>
   </si>
@@ -78,6 +78,24 @@
   </si>
   <si>
     <t>As a manager I want to be able to see reports on hours worked by user</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Med</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>Liam</t>
   </si>
 </sst>
 </file>
@@ -432,87 +450,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A653B9-5D5A-45CC-8550-4BF71F68E3AA}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="77.26953125" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>